<commit_message>
code for post method
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_UserSkills.xlsx
+++ b/src/test/resources/TestData/InputData_UserSkills.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{58F6CD44-2D29-4EFD-BE77-AB187BACC095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{82BD690A-82A6-45CF-8F83-6932BEB05D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="23304" windowHeight="13224" activeTab="1" xr2:uid="{66CCB3E7-3A9B-41B0-9BFC-43F22BA27510}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17520" windowHeight="13224" activeTab="1" xr2:uid="{66CCB3E7-3A9B-41B0-9BFC-43F22BA27510}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData_UserSkills_GET" sheetId="1" r:id="rId1"/>
     <sheet name="InputData_UserSkills_POST" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:N9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>UserSkills_ID</t>
   </si>
@@ -72,31 +72,67 @@
     <t>StatusMessage</t>
   </si>
   <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>Skill_id</t>
+  </si>
+  <si>
+    <t>months_of_exp</t>
+  </si>
+  <si>
+    <t>Senario</t>
+  </si>
+  <si>
+    <t>Successfully Created</t>
+  </si>
+  <si>
     <t>user_skill_id</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>Skill_id</t>
-  </si>
-  <si>
-    <t>months_of_exp</t>
-  </si>
-  <si>
-    <t>Senario</t>
+    <t>U04</t>
+  </si>
+  <si>
+    <t>US15</t>
   </si>
   <si>
     <t>To map new user and skill</t>
   </si>
   <si>
-    <t>Successfully Created</t>
-  </si>
-  <si>
-    <t>U09</t>
-  </si>
-  <si>
-    <t>U10</t>
+    <t>To map new user and skill , with skill id as alpha numeric</t>
+  </si>
+  <si>
+    <t>To map new user and skill , with skill id as null</t>
+  </si>
+  <si>
+    <t>To map new user and skill , with user id as null</t>
+  </si>
+  <si>
+    <t>U07</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>To map new user and skill , with months of experience as alpha numeric</t>
+  </si>
+  <si>
+    <t>To map new user and skill , with months of experience as null</t>
+  </si>
+  <si>
+    <t>a11</t>
+  </si>
+  <si>
+    <t>Failed to create due to invalid data</t>
+  </si>
+  <si>
+    <t>To map to existing user And Skills</t>
+  </si>
+  <si>
+    <t>Failed to create as UserSkillMap already exists</t>
+  </si>
+  <si>
+    <t>Failed to create due to invalid skill Id</t>
   </si>
 </sst>
 </file>
@@ -106,7 +142,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,9 +159,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,10 +186,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -472,16 +508,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -495,7 +531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -506,7 +542,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -520,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -534,7 +570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -548,7 +584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -562,7 +598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -583,34 +619,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2C2F01-0E67-471F-B131-6F010A088F24}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -619,47 +655,143 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>201</v>
       </c>
       <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
       <c r="D3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>201</v>
+        <v>400</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
-      </c>
-    </row>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>400</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>400</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>400</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>400</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>400</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Json Schemas for user Skill
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_UserSkills.xlsx
+++ b/src/test/resources/TestData/InputData_UserSkills.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B494CD0C-D880-48DB-99AF-94B2E10F91A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FF4FF89B-83BE-4422-B413-9F3EB3DF58A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="20076" windowHeight="13224" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="20100" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData_UserSkills_GET" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="InputData_UserSkills_DELETE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H11"/>
+  <oleSize ref="A1:K20"/>
 </workbook>
 </file>
 
@@ -605,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
feture file & step def file changed for userSkills
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_UserSkills.xlsx
+++ b/src/test/resources/TestData/InputData_UserSkills.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{00B6ADEB-EA40-4B4B-A066-214BC8B61F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{66AB4468-1E1F-4A81-A319-E92BAE3376AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="20268" windowHeight="13224" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="20316" windowHeight="13224" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData_UserSkills_GET" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="InputData_UserSkills_DELETE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I6"/>
+  <oleSize ref="A1:E4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Scenario</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Successfully deleted</t>
   </si>
   <si>
-    <t>User Skill Map Not Found</t>
-  </si>
-  <si>
     <t>US20.21</t>
   </si>
   <si>
@@ -208,6 +205,12 @@
   </si>
   <si>
     <t>Failed to update due to invalid months of experience</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>User skill Map Not Found</t>
   </si>
 </sst>
 </file>
@@ -764,7 +767,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>30</v>
@@ -784,11 +787,11 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4">
         <v>4</v>
@@ -800,7 +803,7 @@
         <v>400</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" customFormat="1" ht="26.4">
@@ -821,12 +824,12 @@
         <v>400</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" customFormat="1" ht="26.4">
       <c r="A5" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -840,7 +843,7 @@
         <v>400</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" customFormat="1">
@@ -859,7 +862,7 @@
         <v>400</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7" customFormat="1">
@@ -878,16 +881,16 @@
         <v>400</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7" customFormat="1" ht="26.4">
       <c r="A8" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="15">
         <v>4</v>
@@ -899,7 +902,7 @@
         <v>400</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" customFormat="1" ht="26.4">
@@ -920,7 +923,7 @@
         <v>400</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" customFormat="1" ht="26.4">
@@ -939,7 +942,7 @@
         <v>400</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -987,7 +990,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3">
         <v>30</v>
@@ -1018,7 +1021,7 @@
     </row>
     <row r="4" spans="1:5" ht="28.8">
       <c r="A4" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -1030,12 +1033,12 @@
         <v>400</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -1047,12 +1050,12 @@
         <v>400</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8">
       <c r="A6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -1064,7 +1067,7 @@
         <v>400</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1076,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1105,10 +1108,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1">
         <v>200</v>
@@ -1119,7 +1122,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1128,48 +1131,48 @@
         <v>404</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <v>404</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1">
         <v>404</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
         <v>404</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in Delete feature file & get feature file of user skill & made respective changes in the in step def & util files
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_UserSkills.xlsx
+++ b/src/test/resources/TestData/InputData_UserSkills.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{74458DF7-AB01-4A52-83FB-F97F5F13B88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5A8EC392-2EF8-4D89-9320-E2F5D837AF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="20340" windowHeight="13224" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="20412" windowHeight="13224" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData_UserSkills_GET" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="InputData_UserSkills_DELETE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E3"/>
+  <oleSize ref="A1:G6"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Scenario</t>
   </si>
@@ -201,16 +201,16 @@
     <t>Failed to update due to invalid months of experience</t>
   </si>
   <si>
+    <t>User skill Map Not Found</t>
+  </si>
+  <si>
+    <t>GET method for non existing UserSkillsID</t>
+  </si>
+  <si>
+    <t>GET method for invalid UserSkillsID</t>
+  </si>
+  <si>
     <t>US17</t>
-  </si>
-  <si>
-    <t>User skill Map Not Found</t>
-  </si>
-  <si>
-    <t>GET method for non existing UserSkillsID</t>
-  </si>
-  <si>
-    <t>GET method for invalid UserSkillsID</t>
   </si>
 </sst>
 </file>
@@ -617,9 +617,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -649,7 +649,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -726,17 +726,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="38.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="38.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -767,7 +767,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>28</v>
@@ -955,17 +955,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="67" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="67.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1080,16 +1080,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1131,7 +1131,7 @@
         <v>404</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1146,7 +1146,7 @@
         <v>404</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1160,7 +1160,7 @@
         <v>404</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1172,7 +1172,7 @@
         <v>404</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes UserSkillsstep def  send Request & lmsApiconstant
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_UserSkills.xlsx
+++ b/src/test/resources/TestData/InputData_UserSkills.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>Scenario</t>
   </si>
@@ -682,9 +682,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -797,11 +797,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="38.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="38.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1026,11 +1026,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="67" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="67.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1150,11 +1150,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1258,7 +1258,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.77734375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="29.4" thickBot="1">

</xml_diff>